<commit_message>
added info to rtm
</commit_message>
<xml_diff>
--- a/RTM Document.xlsx
+++ b/RTM Document.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2302c04623c2e868/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aflem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E15EFCE-E1F9-4299-BD7E-6468319F01F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EEF711-AFA9-4FF1-9EBE-7CEB9F7FDE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DFD0881F-4B80-4965-9D29-C12E8850B0ED}"/>
+    <workbookView xWindow="4185" yWindow="1755" windowWidth="21600" windowHeight="11835" xr2:uid="{DFD0881F-4B80-4965-9D29-C12E8850B0ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
-  <si>
-    <t>Requirements Traceability Matrix</t>
-  </si>
-  <si>
-    <t>Employee Reimbursement System</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
   <si>
     <t>Feature/Requirment</t>
   </si>
@@ -82,18 +76,9 @@
     <t>(1.1)Scenario: Login With Correct Credentials</t>
   </si>
   <si>
-    <t>1.1 Pass, 1.2 Pass</t>
-  </si>
-  <si>
-    <t>1.1 PASS, 1.2 fale</t>
-  </si>
-  <si>
     <t>Incomplete</t>
   </si>
   <si>
-    <t>Eric Suminski</t>
-  </si>
-  <si>
     <t>Manager login</t>
   </si>
   <si>
@@ -118,21 +103,12 @@
     <t>Manager should be able logout</t>
   </si>
   <si>
-    <t>View request</t>
-  </si>
-  <si>
     <t>Manager should view request</t>
   </si>
   <si>
-    <t>Approve request</t>
-  </si>
-  <si>
     <t>Manager should approve request</t>
   </si>
   <si>
-    <t>Deny request</t>
-  </si>
-  <si>
     <t>Manager should deny request</t>
   </si>
   <si>
@@ -148,41 +124,146 @@
     <t>Employee should view request</t>
   </si>
   <si>
-    <t>Scenario: Logout with button</t>
-  </si>
-  <si>
-    <t>Scenario: Logout button error</t>
-  </si>
-  <si>
-    <t>Scenario: Table load</t>
-  </si>
-  <si>
-    <t>Scenario: Submit Approve</t>
-  </si>
-  <si>
-    <t>Scenario: Submit Deny</t>
-  </si>
-  <si>
-    <t>Scenario: Table load failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenario: Submit Approve failed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenario: Submit Deny failed </t>
-  </si>
-  <si>
-    <t>Scenario: Create request</t>
-  </si>
-  <si>
-    <t>Scenario: request create failed</t>
+    <t>Requirement Traceability Matrix</t>
+  </si>
+  <si>
+    <t>Manager view request</t>
+  </si>
+  <si>
+    <t>Manager deny request</t>
+  </si>
+  <si>
+    <t>()Scenario: Login With Correct Credentials</t>
+  </si>
+  <si>
+    <t>()Scenario: Login with incorrect credentials</t>
+  </si>
+  <si>
+    <t>()Scenario: Logout with button</t>
+  </si>
+  <si>
+    <t>()Scenario: Table load</t>
+  </si>
+  <si>
+    <t>()Scenario: Submit Approve</t>
+  </si>
+  <si>
+    <t>()Scenario: Submit Deny</t>
+  </si>
+  <si>
+    <t>()Scenario: Create request</t>
+  </si>
+  <si>
+    <t>()Scenario: Logout button error</t>
+  </si>
+  <si>
+    <t>()Scenario: Table load failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">()Scenario: Submit Approve failed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">()Scenario: Submit Deny failed </t>
+  </si>
+  <si>
+    <t>()Scenario: request create failed</t>
+  </si>
+  <si>
+    <t>Manager approve request</t>
+  </si>
+  <si>
+    <t>Employee sees their requests</t>
+  </si>
+  <si>
+    <t>Employees request no longer than 500 Char</t>
+  </si>
+  <si>
+    <t>Managers reason no longer than 500 Char</t>
+  </si>
+  <si>
+    <t>Employee must only see their requests</t>
+  </si>
+  <si>
+    <t>Employee request up to $1000</t>
+  </si>
+  <si>
+    <t>Employees may only request upto $1000</t>
+  </si>
+  <si>
+    <t>Employee request is no more than 500 characters</t>
+  </si>
+  <si>
+    <t>Managers approve or denial reason is no more than 500 characters</t>
+  </si>
+  <si>
+    <t>Managers usernames must be unique</t>
+  </si>
+  <si>
+    <t>Employees usernames must be unique</t>
+  </si>
+  <si>
+    <t>Employees must have unique usernames</t>
+  </si>
+  <si>
+    <t>Managers must have unique usernames</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria</t>
+  </si>
+  <si>
+    <t>()Scenario: Sees others requests</t>
+  </si>
+  <si>
+    <t>()Scenario: Makes over 1000$ requests</t>
+  </si>
+  <si>
+    <t>()Scenario: Sees only their requests</t>
+  </si>
+  <si>
+    <t>()Scenario: Makes up 1000$ requests</t>
+  </si>
+  <si>
+    <t>()Scenario: Request is no more than 500 characters</t>
+  </si>
+  <si>
+    <t>()Scenario: Manager approval or denial is no more than 500 character</t>
+  </si>
+  <si>
+    <t>()Scenraio: Managers have unique usernames</t>
+  </si>
+  <si>
+    <t>()Scenario: Employees have unique usernames</t>
+  </si>
+  <si>
+    <t>()Scenario: Request is more than 500 characters</t>
+  </si>
+  <si>
+    <t>()Scenario: Manager approval or denial is more than 500 characters</t>
+  </si>
+  <si>
+    <t>()Scenraio: Managers do not have unique usernames</t>
+  </si>
+  <si>
+    <t>()Scenraio: Employees do not have unique usernames</t>
+  </si>
+  <si>
+    <t>Seble</t>
+  </si>
+  <si>
+    <t>Sherrita</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Richard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,12 +284,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -244,13 +319,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,31 +639,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439A12EF-3E90-4D33-94B5-26CA4D060C9D}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="0.109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="6" max="6" width="36.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="44" customWidth="1"/>
-    <col min="10" max="10" width="35.33203125" customWidth="1"/>
-    <col min="11" max="11" width="42.109375" customWidth="1"/>
-    <col min="12" max="12" width="35.44140625" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="15" max="15" width="26" customWidth="1"/>
-    <col min="17" max="17" width="26.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="62.28515625" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -599,58 +668,32 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" ht="21.6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -660,210 +703,379 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" t="s">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="S6" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
         <v>13</v>
       </c>
       <c r="I7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="M7" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>29</v>
+      <c r="C12" t="s">
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
       </c>
       <c r="I14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="K14" t="s">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>46</v>
       </c>
-      <c r="Q14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>17</v>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
constraints to database and test plan updates
</commit_message>
<xml_diff>
--- a/RTM Document.xlsx
+++ b/RTM Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307D0B04-7A73-42A1-954B-DF8466F88D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B304ED21-3D0D-43AA-914A-BC572466EE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="15345" xr2:uid="{DFD0881F-4B80-4965-9D29-C12E8850B0ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DFD0881F-4B80-4965-9D29-C12E8850B0ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>Employee create request</t>
   </si>
   <si>
-    <t>Employee should creat request</t>
-  </si>
-  <si>
     <t>Employee view request</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>Jason</t>
+  </si>
+  <si>
+    <t>Employee should create request</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -825,10 +825,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
@@ -871,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -885,16 +885,16 @@
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -908,16 +908,16 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -931,10 +931,10 @@
         <v>13</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -942,12 +942,12 @@
         <v>10</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>19</v>
@@ -956,10 +956,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -967,12 +967,12 @@
         <v>10</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
@@ -981,21 +981,21 @@
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>21</v>
@@ -1004,10 +1004,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -1015,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1023,16 +1023,16 @@
         <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1040,24 +1040,24 @@
         <v>10</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -1065,24 +1065,24 @@
         <v>10</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1090,93 +1090,93 @@
         <v>10</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="C19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1184,7 +1184,7 @@
         <v>10</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
one method for business rules
</commit_message>
<xml_diff>
--- a/RTM Document.xlsx
+++ b/RTM Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DAFE9E-5E17-45DB-9A7F-BDAB73FE6FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD904200-6E6F-47A7-9A36-2E1204AE409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DFD0881F-4B80-4965-9D29-C12E8850B0ED}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>Feature/Requirment</t>
   </si>
@@ -260,7 +260,16 @@
     <t>(5.1)Scenario: Table load / get all requests</t>
   </si>
   <si>
-    <t>unit?</t>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Ausin</t>
+  </si>
+  <si>
+    <t>Richard</t>
   </si>
 </sst>
 </file>
@@ -438,45 +447,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,7 +816,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,50 +834,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -908,28 +915,25 @@
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" s="18" t="s">
+      <c r="I6" s="10"/>
+      <c r="K6" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -937,28 +941,25 @@
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="18" t="s">
+      <c r="I7" s="11"/>
+      <c r="K7" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -966,25 +967,25 @@
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="K8" s="18" t="s">
+      <c r="I8" s="13"/>
+      <c r="K8" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -992,25 +993,25 @@
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="K9" s="18" t="s">
+      <c r="I9" s="13"/>
+      <c r="K9" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1018,30 +1019,30 @@
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>64</v>
       </c>
       <c r="J10" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1049,30 +1050,30 @@
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="13" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>65</v>
       </c>
       <c r="J11" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1080,30 +1081,30 @@
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="13" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>65</v>
       </c>
       <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1111,28 +1112,25 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" t="s">
-        <v>71</v>
-      </c>
-      <c r="K13" s="18" t="s">
+      <c r="I13" s="11"/>
+      <c r="K13" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1140,30 +1138,30 @@
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="13" t="s">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>64</v>
       </c>
       <c r="J14" t="s">
         <v>71</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1171,28 +1169,25 @@
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8" t="s">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" s="18" t="s">
+      <c r="I15" s="11"/>
+      <c r="K15" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1200,28 +1195,30 @@
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="13"/>
+      <c r="I16" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="J16" t="s">
         <v>72</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1229,28 +1226,30 @@
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="13"/>
+      <c r="I17" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="J17" t="s">
         <v>72</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1258,57 +1257,61 @@
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="13"/>
+      <c r="I18" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="J18" t="s">
         <v>72</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" t="s">
+      <c r="I19" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="7" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
logout method added to requester pom
</commit_message>
<xml_diff>
--- a/RTM Document.xlsx
+++ b/RTM Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CF3186-4AE5-4212-965B-7006DF80915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF4ECC8-D1F5-4C64-A5C6-480FA601C90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DFD0881F-4B80-4965-9D29-C12E8850B0ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>Feature/Requirment</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>automated results</t>
-  </si>
-  <si>
-    <t>Overall Stauts</t>
   </si>
   <si>
     <t>Assigned To</t>
@@ -111,9 +108,6 @@
     <t>BR3.2.2 request reason should not exceed 500 characters</t>
   </si>
   <si>
-    <t>1. employees should be able to log in to role page</t>
-  </si>
-  <si>
     <t>2. managers should view and update request status</t>
   </si>
   <si>
@@ -276,21 +270,6 @@
     <t>1.1s: m-credentials invalid</t>
   </si>
   <si>
-    <t>4. employees should be able to log out</t>
-  </si>
-  <si>
-    <t>1.1 requester logs out to login page</t>
-  </si>
-  <si>
-    <t>1.2 manager logs out to login page</t>
-  </si>
-  <si>
-    <t>4.1 requester page log out button leads to log in page</t>
-  </si>
-  <si>
-    <t>4.2 manager page log out button leads to log in page</t>
-  </si>
-  <si>
     <t>Quyen and Richard</t>
   </si>
   <si>
@@ -306,7 +285,22 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>r</t>
+    <t>Overall Status</t>
+  </si>
+  <si>
+    <t>1. employees should be able to log in to role page and log out to login page</t>
+  </si>
+  <si>
+    <t>1.3 requester logs out to login page</t>
+  </si>
+  <si>
+    <t>1.4 manager logs out to login page</t>
+  </si>
+  <si>
+    <t>1.3e: requester logs out of role page to login page</t>
+  </si>
+  <si>
+    <t>1.4e: manager logs out of manager page to login page</t>
   </si>
 </sst>
 </file>
@@ -446,9 +440,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -475,25 +466,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,15 +836,15 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -862,68 +856,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="A1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>1</v>
@@ -938,491 +932,487 @@
         <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="J5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>13</v>
+      <c r="A6" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="3"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="23"/>
       <c r="E8" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I8" s="24"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="3"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="15"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="I9" s="24"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="3"/>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="16"/>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="3"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="15" t="s">
-        <v>19</v>
+      <c r="A12" s="20"/>
+      <c r="B12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="I14" s="24"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
+    <row r="15" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="18"/>
+      <c r="I16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="15"/>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="I17" s="24"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="3"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>62</v>
+      <c r="A18" s="20"/>
+      <c r="B18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="3"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="10"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>64</v>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="24"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="H20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>41</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="22"/>
-      <c r="D21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>65</v>
+    <row r="21" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>63</v>
+      <c r="A23" s="20"/>
+      <c r="B23" s="23"/>
+      <c r="D23" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I23" s="24"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="3"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="18"/>
+      <c r="H24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="24"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="3"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="C25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>67</v>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="I25" s="24"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="3"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="10"/>
-    </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="C26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="C27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="H27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="19"/>
+    <row r="28" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -1605,24 +1595,22 @@
       <c r="L41" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="15">
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="I6:I14"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A6:A14"/>
     <mergeCell ref="J6:J11"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="J20:J25"/>
+    <mergeCell ref="J16:J20"/>
+    <mergeCell ref="J22:J27"/>
     <mergeCell ref="A1:K4"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A22:A27"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="I20:I25"/>
-    <mergeCell ref="I6:I12"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H29">
     <cfRule type="beginsWith" dxfId="3" priority="3" operator="beginsWith" text="Complete">
@@ -1661,138 +1649,138 @@
   <sheetData>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D15" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D16" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>